<commit_message>
Correccion de mando para llevar y enviar datos de inventario
</commit_message>
<xml_diff>
--- a/productosV2.xlsx
+++ b/productosV2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairo\Documents\Chumazero_Ambato\ChumaBot\Bot_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264A2F17-691A-408E-A3E8-678F8C1E0D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61566CE9-C7E8-428B-8B1A-C689B02BC64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="426">
   <si>
     <t>name</t>
   </si>
@@ -1309,6 +1309,9 @@
   </si>
   <si>
     <t>Zhumir Mango</t>
+  </si>
+  <si>
+    <t>Zhumir M TG</t>
   </si>
 </sst>
 </file>
@@ -1686,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1904,7 +1907,7 @@
       <c r="G7" t="s">
         <v>421</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>197</v>
       </c>
       <c r="I7">
@@ -3755,12 +3758,12 @@
         <v>223</v>
       </c>
       <c r="B71" t="s">
-        <v>122</v>
+        <v>425</v>
       </c>
       <c r="C71">
         <v>5.5</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="3" t="s">
         <v>424</v>
       </c>
       <c r="E71" t="s">
@@ -7344,7 +7347,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61FC2263-E473-4073-9BC9-993B02413194}">
           <x14:formula1>
             <xm:f>Hoja1!$B$2:$B$95</xm:f>

</xml_diff>

<commit_message>
Actualizacion de precios smirnoff
</commit_message>
<xml_diff>
--- a/productosV2.xlsx
+++ b/productosV2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairo\Documents\Chumazero_Ambato\ChumaBot\Bot_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61566CE9-C7E8-428B-8B1A-C689B02BC64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EA93F8-9B71-4F7B-9C66-70B0AD05F887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1318,7 +1318,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1341,6 +1341,14 @@
       <sz val="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1384,7 +1392,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1689,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3101,7 +3109,7 @@
         <v>362</v>
       </c>
       <c r="C49">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D49" t="s">
         <v>362</v>
@@ -3130,7 +3138,7 @@
       <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="3">
         <v>3.5</v>
       </c>
       <c r="D50" t="s">
@@ -3763,7 +3771,7 @@
       <c r="C71">
         <v>5.5</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" t="s">
         <v>424</v>
       </c>
       <c r="E71" t="s">

</xml_diff>